<commit_message>
Remade lost data, added excel explanation for formatting
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Nezic\IdeaProjects\CucumberIAG\src\test\java\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B3D95D-711C-4E66-8285-91B55209B7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9B6142-90A4-4EC5-918C-8B950D42609E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Flight Type</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Departure Date</t>
   </si>
   <si>
-    <t>Arrival Date</t>
-  </si>
-  <si>
     <t>Adults</t>
   </si>
   <si>
@@ -82,6 +79,45 @@
   </si>
   <si>
     <t>Multi Destination Date 3</t>
+  </si>
+  <si>
+    <t>Oneway</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Multi</t>
+  </si>
+  <si>
+    <t>Melbourne</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>Tasmania</t>
+  </si>
+  <si>
+    <t>Adelaide</t>
+  </si>
+  <si>
+    <t>Hobart</t>
+  </si>
+  <si>
+    <t>Return Date</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>First Class</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Premium Economy</t>
   </si>
 </sst>
 </file>
@@ -125,10 +161,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -444,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354668D4-D94F-4400-B0BC-72EF38E5F017}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A2" sqref="A2:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +499,7 @@
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.140625" bestFit="1" customWidth="1"/>
@@ -486,38 +525,279 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2">
+        <v>25012022</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
+        <v>25022022</v>
+      </c>
+      <c r="F3" s="2">
+        <v>27022022</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2">
+        <v>25012022</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>4</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="2">
+        <v>27012022</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="2">
+        <v>28012022</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2">
+        <v>25012022</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2">
+        <v>25022022</v>
+      </c>
+      <c r="F6" s="2">
+        <v>27022022</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2">
+        <v>25012022</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="2">
+        <v>27012022</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bug fixes in regex for validation, bug fix for incorrect return date month when departure month is not current month
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Nezic\IdeaProjects\CucumberIAG\src\test\java\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4DD25D-FBB6-4588-8ACC-53DAB668EA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A25542-F60A-4E93-A936-4266225A94F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
   <si>
     <t>Flight Type</t>
   </si>
@@ -127,19 +127,22 @@
     <t>Message</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Arrival location 1 does not match dataset</t>
+  </si>
+  <si>
+    <t>No flight results</t>
+  </si>
+  <si>
+    <t>Entry</t>
+  </si>
+  <si>
     <t>N</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Arrival location 1 does not match dataset</t>
-  </si>
-  <si>
-    <t>No flight results</t>
   </si>
 </sst>
 </file>
@@ -191,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,6 +202,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,249 +530,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354668D4-D94F-4400-B0BC-72EF38E5F017}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
-    <col min="8" max="8" style="2" width="9.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="7.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="2" width="19.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="18.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="23.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
-    <col min="17" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="18.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="23.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
+    <col min="18" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>25012022</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3">
         <v>3</v>
       </c>
-      <c r="H2" s="3">
-        <v>1</v>
-      </c>
       <c r="I2" s="3">
         <v>1</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>25022022</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>27022022</v>
       </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
       <c r="H3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="3">
         <v>0</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3">
+      <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>25012022</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="6"/>
+      <c r="H4" s="3">
         <v>2</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>4</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>0</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>27012022</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>28012022</v>
       </c>
-      <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="Q4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>25012022</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
+      <c r="G5" s="3"/>
       <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
         <v>0</v>
       </c>
-      <c r="I5" s="3">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>25022022</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>27022022</v>
-      </c>
-      <c r="G6" s="3">
-        <v>2</v>
       </c>
       <c r="H6" s="3">
         <v>2</v>
@@ -764,57 +796,63 @@
       <c r="I6" s="3">
         <v>2</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="3">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>25012022</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="3">
         <v>1</v>
       </c>
       <c r="I7" s="3">
         <v>1</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="3">
         <v>27012022</v>
       </c>
-      <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -831,6 +869,25 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
+      <c r="Q8" s="6"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -840,28 +897,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116CE802-AF6A-49F4-92A0-B86909AD8334}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="40.7109375" collapsed="true"/>
-    <col min="3" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="46.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="40.85546875" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="C1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
@@ -869,19 +930,63 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s">
-        <v>33</v>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Timestamp addition to excel output
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Nezic\IdeaProjects\CucumberIAG\src\test\java\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A25542-F60A-4E93-A936-4266225A94F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F852705E-84FE-4EBB-859E-59DB64D912DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Flight Type</t>
   </si>
@@ -127,22 +127,13 @@
     <t>Message</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Arrival location 1 does not match dataset</t>
-  </si>
-  <si>
-    <t>No flight results</t>
-  </si>
-  <si>
     <t>Entry</t>
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>18/01/2022 3:11:03 pm - 18/01/2022 3:10:58 pm</t>
   </si>
 </sst>
 </file>
@@ -532,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354668D4-D94F-4400-B0BC-72EF38E5F017}">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -559,7 +550,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -899,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116CE802-AF6A-49F4-92A0-B86909AD8334}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -922,51 +913,31 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7"/>
+      <c r="B7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>

</xml_diff>

<commit_message>
- Overloaded setData function to accommodate String array for booking price values to be exported - Added functionality for all flight types to have their fare values exported into excel - Added additional exception handling for wait elements (in case they don't load) - Rearranged Excel spreadsheet to accommodate additional data output - Added comments for datepicker method as it is complicated to understand
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Nezic\IdeaProjects\CucumberIAG\src\test\java\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F852705E-84FE-4EBB-859E-59DB64D912DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3D7C3F-71F2-460B-AD6A-9958BA3814D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>Flight Type</t>
   </si>
@@ -130,17 +130,94 @@
     <t>Entry</t>
   </si>
   <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Base Fare</t>
+  </si>
+  <si>
+    <t>Fee/Surcharge</t>
+  </si>
+  <si>
+    <t>Addons</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>18/01/2022 3:11:03 pm - 18/01/2022 3:10:58 pm</t>
+    <t>₹1,21,420</t>
+  </si>
+  <si>
+    <t>₹8,332</t>
+  </si>
+  <si>
+    <t>₹10</t>
+  </si>
+  <si>
+    <t>₹1,29,762</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Arrival location 1 does not match dataset</t>
+  </si>
+  <si>
+    <t>Fare elements not found</t>
+  </si>
+  <si>
+    <t>No flight results</t>
+  </si>
+  <si>
+    <t>19/01/2022 11:43:05 am</t>
+  </si>
+  <si>
+    <t>19/01/2022 11:43:12 am</t>
+  </si>
+  <si>
+    <t>19/01/2022 11:43:39 am</t>
+  </si>
+  <si>
+    <t>1,018,020</t>
+  </si>
+  <si>
+    <t>38,556</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>868,618</t>
+  </si>
+  <si>
+    <t>19/01/2022 11:44:07 am</t>
+  </si>
+  <si>
+    <t>19/01/2022 11:45:11 am</t>
+  </si>
+  <si>
+    <t>19/01/2022 11:45:32 am</t>
+  </si>
+  <si>
+    <t>97,330</t>
+  </si>
+  <si>
+    <t>8,938</t>
+  </si>
+  <si>
+    <t>106,274</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -529,23 +606,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="11.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="18.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="23.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
-    <col min="18" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -888,73 +965,165 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116CE802-AF6A-49F4-92A0-B86909AD8334}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="A2:B7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="46.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="40.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2">
+      <c r="D1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>

</xml_diff>

<commit_message>
- General code tidy + debugging - Added check for empty row - Added capacity of 10 Excel rows that can be tested at once
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Nezic\IdeaProjects\CucumberIAG\src\test\java\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3D7C3F-71F2-460B-AD6A-9958BA3814D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D37606-03C8-4A15-A1DA-23F11C91C216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
   <si>
     <t>Flight Type</t>
   </si>
@@ -148,18 +148,9 @@
     <t>N</t>
   </si>
   <si>
-    <t>₹1,21,420</t>
-  </si>
-  <si>
-    <t>₹8,332</t>
-  </si>
-  <si>
     <t>₹10</t>
   </si>
   <si>
-    <t>₹1,29,762</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -169,49 +160,88 @@
     <t>Arrival location 1 does not match dataset</t>
   </si>
   <si>
-    <t>Fare elements not found</t>
-  </si>
-  <si>
     <t>No flight results</t>
   </si>
   <si>
-    <t>19/01/2022 11:43:05 am</t>
-  </si>
-  <si>
-    <t>19/01/2022 11:43:12 am</t>
-  </si>
-  <si>
-    <t>19/01/2022 11:43:39 am</t>
-  </si>
-  <si>
-    <t>1,018,020</t>
-  </si>
-  <si>
-    <t>38,556</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
-    <t>868,618</t>
-  </si>
-  <si>
-    <t>19/01/2022 11:44:07 am</t>
-  </si>
-  <si>
-    <t>19/01/2022 11:45:11 am</t>
-  </si>
-  <si>
-    <t>19/01/2022 11:45:32 am</t>
-  </si>
-  <si>
-    <t>97,330</t>
-  </si>
-  <si>
-    <t>8,938</t>
-  </si>
-  <si>
-    <t>106,274</t>
+    <t>₹1,21,500</t>
+  </si>
+  <si>
+    <t>₹8,344</t>
+  </si>
+  <si>
+    <t>₹1,29,854</t>
+  </si>
+  <si>
+    <t>901,890</t>
+  </si>
+  <si>
+    <t>38,610</t>
+  </si>
+  <si>
+    <t>940,510</t>
+  </si>
+  <si>
+    <t>97,390</t>
+  </si>
+  <si>
+    <t>8,954</t>
+  </si>
+  <si>
+    <t>106,354</t>
+  </si>
+  <si>
+    <t>₹1,44,270</t>
+  </si>
+  <si>
+    <t>₹10,324</t>
+  </si>
+  <si>
+    <t>₹1,54,604</t>
+  </si>
+  <si>
+    <t>20/01/2022 12:17:08 pm</t>
+  </si>
+  <si>
+    <t>20/01/2022 12:17:20 pm</t>
+  </si>
+  <si>
+    <t>20/01/2022 12:17:33 pm</t>
+  </si>
+  <si>
+    <t>20/01/2022 12:17:42 pm</t>
+  </si>
+  <si>
+    <t>20/01/2022 12:17:59 pm</t>
+  </si>
+  <si>
+    <t>20/01/2022 12:18:12 pm</t>
+  </si>
+  <si>
+    <t>20/01/2022 12:18:27 pm</t>
+  </si>
+  <si>
+    <t>Autosuggest element for departure location not found. Timeout</t>
+  </si>
+  <si>
+    <t>20/01/2022 12:18:32 pm</t>
+  </si>
+  <si>
+    <t>Row 8 does not exist</t>
+  </si>
+  <si>
+    <t>20/01/2022 12:18:37 pm</t>
+  </si>
+  <si>
+    <t>Row 9 does not exist</t>
+  </si>
+  <si>
+    <t>20/01/2022 12:18:46 pm</t>
+  </si>
+  <si>
+    <t>Row 10 does not exist</t>
   </si>
 </sst>
 </file>
@@ -281,8 +311,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354668D4-D94F-4400-B0BC-72EF38E5F017}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -920,43 +950,6 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="6"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -968,7 +961,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1008,125 +1001,161 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
-        <v>41</v>
+      <c r="C2" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>39</v>
-      </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="C4" t="s">
-        <v>41</v>
+      <c r="C4" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
         <v>54</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
-        <v>41</v>
+      <c r="C7" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s">
         <v>51</v>
       </c>
-      <c r="G7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Removed redundant variable for 'row' in FlightStep and Goibibo to reduce code - Added new exception for flight type not being found - Reformatted lines in all files
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Nezic\IdeaProjects\CucumberIAG\src\test\java\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D37606-03C8-4A15-A1DA-23F11C91C216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8378B52F-8D8F-46AF-9491-7B13A66707A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
   </bookViews>
@@ -202,9 +202,6 @@
     <t>₹1,54,604</t>
   </si>
   <si>
-    <t>20/01/2022 12:17:08 pm</t>
-  </si>
-  <si>
     <t>20/01/2022 12:17:20 pm</t>
   </si>
   <si>
@@ -242,6 +239,9 @@
   </si>
   <si>
     <t>Row 10 does not exist</t>
+  </si>
+  <si>
+    <t>20/01/2022 2:31:39 pm</t>
   </si>
 </sst>
 </file>
@@ -961,7 +961,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1001,12 +1001,12 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>38</v>
       </c>
       <c r="D2" t="s">
@@ -1024,7 +1024,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
@@ -1115,46 +1115,46 @@
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enabled screenshot utility (previously present, just not used), updated filepath to new folder and changed filetype bmp -> jpeg
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Nezic\IdeaProjects\CucumberIAG\src\test\java\Excel\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
   <si>
     <t>Flight Type</t>
   </si>
@@ -242,12 +242,28 @@
   </si>
   <si>
     <t>20/01/2022 2:31:39 pm</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:19:49 am</t>
+  </si>
+  <si>
+    <t>₹1,21,740</t>
+  </si>
+  <si>
+    <t>₹8,356</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:23:32 am</t>
+  </si>
+  <si>
+    <t>₹1,30,106</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -636,23 +652,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="18.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="23.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
+    <col min="18" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -966,14 +982,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="21.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="7.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="37.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="16.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="16.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="15.7109375" collapsed="true"/>
+    <col min="8" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -999,9 +1015,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -1010,16 +1026,16 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s">
         <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Added new step in feature file to break up code and make more logical sense - Updated page source check to see if correct page shows, as incorrect webpage now sometimes displays elements from both versions (idk what's going on here) - Fixed switch for flight type, forgot return in final case - Updated screenshot utility to create new folders to organise screenshots better (titled by date and hour)
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="104">
   <si>
     <t>Flight Type</t>
   </si>
@@ -257,6 +257,96 @@
   </si>
   <si>
     <t>₹1,30,106</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:38:36 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:44:42 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:44:54 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:45:00 am</t>
+  </si>
+  <si>
+    <t>Flight type not found</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:45:14 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:45:46 am</t>
+  </si>
+  <si>
+    <t>Fare elements not found. Timeout</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:45:51 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:46:34 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:46:40 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:46:50 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:47:56 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:48:15 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:48:26 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:48:55 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:49:18 am</t>
+  </si>
+  <si>
+    <t>₹1,44,570</t>
+  </si>
+  <si>
+    <t>₹10,340</t>
+  </si>
+  <si>
+    <t>₹1,54,920</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:51:31 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:51:43 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:51:48 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:59:26 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 11:59:33 am</t>
+  </si>
+  <si>
+    <t>21/01/2022 12:00:21 pm</t>
+  </si>
+  <si>
+    <t>21/01/2022 12:00:28 pm</t>
+  </si>
+  <si>
+    <t>21/01/2022 12:01:01 pm</t>
+  </si>
+  <si>
+    <t>21/01/2022 12:01:09 pm</t>
+  </si>
+  <si>
+    <t>21/01/2022 12:01:22 pm</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1107,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -1038,95 +1128,71 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" t="s">
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
         <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" t="s">
-        <v>51</v>
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes for Cucumber Reporting in Jenkins
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="142">
   <si>
     <t>Flight Type</t>
   </si>
@@ -359,6 +359,108 @@
   </si>
   <si>
     <t>21/01/2022 2:35:26 pm</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:05:08 pm</t>
+  </si>
+  <si>
+    <t>₹1,22,140</t>
+  </si>
+  <si>
+    <t>₹8,368</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:06:59 pm</t>
+  </si>
+  <si>
+    <t>₹1,30,518</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:07:17 pm</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:07:49 pm</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:08:16 pm</t>
+  </si>
+  <si>
+    <t>₹1,45,040</t>
+  </si>
+  <si>
+    <t>₹10,360</t>
+  </si>
+  <si>
+    <t>₹1,55,410</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:08:41 pm</t>
+  </si>
+  <si>
+    <t>97,900</t>
+  </si>
+  <si>
+    <t>8,980</t>
+  </si>
+  <si>
+    <t>106,890</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:08:52 pm</t>
+  </si>
+  <si>
+    <t>Row 6 is empty</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:09:02 pm</t>
+  </si>
+  <si>
+    <t>Row 7 does not exist</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:09:07 pm</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:09:12 pm</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:23:53 pm</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:24:00 pm</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:24:42 pm</t>
+  </si>
+  <si>
+    <t>1,032,360</t>
+  </si>
+  <si>
+    <t>41,082</t>
+  </si>
+  <si>
+    <t>1,073,452</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:24:51 pm</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:25:03 pm</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:25:18 pm</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:25:33 pm</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:25:38 pm</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:25:43 pm</t>
+  </si>
+  <si>
+    <t>23/01/2022 2:25:48 pm</t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1221,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -1128,21 +1230,21 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="F2" t="s">
         <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
@@ -1153,18 +1255,30 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -1175,7 +1289,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -1184,71 +1298,83 @@
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="F6" t="s">
         <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>138</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>67</v>
+      <c r="C11" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Updated Picocontainer - Added Page Object Models for Homepage and Flight Selection pages. Transferred code from Steps to respective page models - Depreciated previous files where necessary - Renamed Goibibo file to better specify purpose - Fixed typos
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="157">
   <si>
     <t>Flight Type</t>
   </si>
@@ -461,6 +461,51 @@
   </si>
   <si>
     <t>23/01/2022 2:25:48 pm</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:11:12 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:12:41 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:15:32 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:17:41 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:17:50 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:22:15 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:22:22 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:22:38 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:22:46 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:22:59 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:23:15 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:23:20 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:23:30 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:23:35 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 11:24:00 am</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1266,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -1244,7 +1289,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
@@ -1255,7 +1300,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
@@ -1278,7 +1323,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -1289,7 +1334,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -1312,7 +1357,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
@@ -1335,7 +1380,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
@@ -1346,7 +1391,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
@@ -1357,7 +1402,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
@@ -1368,7 +1413,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="B11" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Updated report file test
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Nezic\IdeaProjects\CucumberIAG\src\test\java\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8378B52F-8D8F-46AF-9491-7B13A66707A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7544F2A-B3F6-4110-8B00-930F4C5944B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
   <si>
     <t>Flight Type</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Sydney</t>
   </si>
   <si>
-    <t>Tasmania</t>
-  </si>
-  <si>
     <t>Adelaide</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>Economy</t>
   </si>
   <si>
-    <t>First Class</t>
-  </si>
-  <si>
     <t>Business</t>
   </si>
   <si>
@@ -166,225 +160,21 @@
     <t>10</t>
   </si>
   <si>
-    <t>₹1,21,500</t>
-  </si>
-  <si>
-    <t>₹8,344</t>
-  </si>
-  <si>
-    <t>₹1,29,854</t>
-  </si>
-  <si>
-    <t>901,890</t>
-  </si>
-  <si>
-    <t>38,610</t>
-  </si>
-  <si>
-    <t>940,510</t>
-  </si>
-  <si>
-    <t>97,390</t>
-  </si>
-  <si>
-    <t>8,954</t>
-  </si>
-  <si>
-    <t>106,354</t>
-  </si>
-  <si>
-    <t>₹1,44,270</t>
-  </si>
-  <si>
-    <t>₹10,324</t>
-  </si>
-  <si>
-    <t>₹1,54,604</t>
-  </si>
-  <si>
-    <t>20/01/2022 12:17:20 pm</t>
-  </si>
-  <si>
-    <t>20/01/2022 12:17:33 pm</t>
-  </si>
-  <si>
-    <t>20/01/2022 12:17:42 pm</t>
-  </si>
-  <si>
-    <t>20/01/2022 12:17:59 pm</t>
-  </si>
-  <si>
-    <t>20/01/2022 12:18:12 pm</t>
-  </si>
-  <si>
-    <t>20/01/2022 12:18:27 pm</t>
-  </si>
-  <si>
-    <t>Autosuggest element for departure location not found. Timeout</t>
-  </si>
-  <si>
-    <t>20/01/2022 12:18:32 pm</t>
-  </si>
-  <si>
     <t>Row 8 does not exist</t>
   </si>
   <si>
-    <t>20/01/2022 12:18:37 pm</t>
-  </si>
-  <si>
     <t>Row 9 does not exist</t>
   </si>
   <si>
-    <t>20/01/2022 12:18:46 pm</t>
-  </si>
-  <si>
-    <t>Row 10 does not exist</t>
-  </si>
-  <si>
-    <t>20/01/2022 2:31:39 pm</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:19:49 am</t>
-  </si>
-  <si>
-    <t>₹1,21,740</t>
-  </si>
-  <si>
-    <t>₹8,356</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:23:32 am</t>
-  </si>
-  <si>
-    <t>₹1,30,106</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:38:36 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:44:42 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:44:54 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:45:00 am</t>
-  </si>
-  <si>
-    <t>Flight type not found</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:45:14 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:45:46 am</t>
-  </si>
-  <si>
-    <t>Fare elements not found. Timeout</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:45:51 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:46:34 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:46:40 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:46:50 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:47:56 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:48:15 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:48:26 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:48:55 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:49:18 am</t>
-  </si>
-  <si>
-    <t>₹1,44,570</t>
-  </si>
-  <si>
-    <t>₹10,340</t>
-  </si>
-  <si>
-    <t>₹1,54,920</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:51:31 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:51:43 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:51:48 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:59:26 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 11:59:33 am</t>
-  </si>
-  <si>
-    <t>21/01/2022 12:00:21 pm</t>
-  </si>
-  <si>
-    <t>21/01/2022 12:00:28 pm</t>
-  </si>
-  <si>
-    <t>21/01/2022 12:01:01 pm</t>
-  </si>
-  <si>
-    <t>21/01/2022 12:01:09 pm</t>
-  </si>
-  <si>
-    <t>21/01/2022 12:01:22 pm</t>
-  </si>
-  <si>
-    <t>21/01/2022 2:34:26 pm</t>
-  </si>
-  <si>
-    <t>21/01/2022 2:34:44 pm</t>
-  </si>
-  <si>
-    <t>21/01/2022 2:35:12 pm</t>
-  </si>
-  <si>
-    <t>21/01/2022 2:35:26 pm</t>
-  </si>
-  <si>
-    <t>23/01/2022 2:05:08 pm</t>
-  </si>
-  <si>
     <t>₹1,22,140</t>
   </si>
   <si>
     <t>₹8,368</t>
   </si>
   <si>
-    <t>23/01/2022 2:06:59 pm</t>
-  </si>
-  <si>
     <t>₹1,30,518</t>
   </si>
   <si>
-    <t>23/01/2022 2:07:17 pm</t>
-  </si>
-  <si>
-    <t>23/01/2022 2:07:49 pm</t>
-  </si>
-  <si>
-    <t>23/01/2022 2:08:16 pm</t>
-  </si>
-  <si>
     <t>₹1,45,040</t>
   </si>
   <si>
@@ -394,9 +184,6 @@
     <t>₹1,55,410</t>
   </si>
   <si>
-    <t>23/01/2022 2:08:41 pm</t>
-  </si>
-  <si>
     <t>97,900</t>
   </si>
   <si>
@@ -406,33 +193,12 @@
     <t>106,890</t>
   </si>
   <si>
-    <t>23/01/2022 2:08:52 pm</t>
-  </si>
-  <si>
     <t>Row 6 is empty</t>
   </si>
   <si>
-    <t>23/01/2022 2:09:02 pm</t>
-  </si>
-  <si>
     <t>Row 7 does not exist</t>
   </si>
   <si>
-    <t>23/01/2022 2:09:07 pm</t>
-  </si>
-  <si>
-    <t>23/01/2022 2:09:12 pm</t>
-  </si>
-  <si>
-    <t>23/01/2022 2:23:53 pm</t>
-  </si>
-  <si>
-    <t>23/01/2022 2:24:00 pm</t>
-  </si>
-  <si>
-    <t>23/01/2022 2:24:42 pm</t>
-  </si>
-  <si>
     <t>1,032,360</t>
   </si>
   <si>
@@ -442,42 +208,6 @@
     <t>1,073,452</t>
   </si>
   <si>
-    <t>23/01/2022 2:24:51 pm</t>
-  </si>
-  <si>
-    <t>23/01/2022 2:25:03 pm</t>
-  </si>
-  <si>
-    <t>23/01/2022 2:25:18 pm</t>
-  </si>
-  <si>
-    <t>23/01/2022 2:25:33 pm</t>
-  </si>
-  <si>
-    <t>23/01/2022 2:25:38 pm</t>
-  </si>
-  <si>
-    <t>23/01/2022 2:25:43 pm</t>
-  </si>
-  <si>
-    <t>23/01/2022 2:25:48 pm</t>
-  </si>
-  <si>
-    <t>24/01/2022 11:11:12 am</t>
-  </si>
-  <si>
-    <t>24/01/2022 11:12:41 am</t>
-  </si>
-  <si>
-    <t>24/01/2022 11:15:32 am</t>
-  </si>
-  <si>
-    <t>24/01/2022 11:17:41 am</t>
-  </si>
-  <si>
-    <t>24/01/2022 11:17:50 am</t>
-  </si>
-  <si>
     <t>24/01/2022 11:22:15 am</t>
   </si>
   <si>
@@ -506,6 +236,24 @@
   </si>
   <si>
     <t>24/01/2022 11:24:00 am</t>
+  </si>
+  <si>
+    <t>24/01/2022 1:40:21 pm</t>
+  </si>
+  <si>
+    <t>24/01/2022 1:40:45 pm</t>
+  </si>
+  <si>
+    <t>₹23,990</t>
+  </si>
+  <si>
+    <t>₹3,761</t>
+  </si>
+  <si>
+    <t>₹27,761</t>
+  </si>
+  <si>
+    <t>24/01/2022 1:41:07 pm</t>
   </si>
 </sst>
 </file>
@@ -557,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -575,9 +323,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -895,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354668D4-D94F-4400-B0BC-72EF38E5F017}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -922,7 +667,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -940,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -1001,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -1022,7 +767,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3">
         <v>25022022</v>
@@ -1040,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -1063,7 +808,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="3">
         <v>25012022</v>
@@ -1079,7 +824,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>19</v>
@@ -1108,7 +853,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3">
         <v>25012022</v>
@@ -1124,7 +869,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -1163,7 +908,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -1186,7 +931,7 @@
         <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="3">
         <v>25012022</v>
@@ -1202,7 +947,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>18</v>
@@ -1225,7 +970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116CE802-AF6A-49F4-92A0-B86909AD8334}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -1243,183 +988,195 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
         <v>42</v>
-      </c>
-      <c r="G4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>154</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>156</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Updated FlightSelection pages to meet Page Object Model formatting (FindBy, etc.) - Begun updating Homepage for same as above
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
   <si>
     <t>Flight Type</t>
   </si>
@@ -254,6 +254,21 @@
   </si>
   <si>
     <t>24/01/2022 1:41:07 pm</t>
+  </si>
+  <si>
+    <t>25/01/2022 1:51:28 pm</t>
+  </si>
+  <si>
+    <t>₹1,21,120</t>
+  </si>
+  <si>
+    <t>₹8,328</t>
+  </si>
+  <si>
+    <t>₹1,29,458</t>
+  </si>
+  <si>
+    <t>25/01/2022 2:23:05 pm</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1026,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
@@ -1020,16 +1035,16 @@
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
         <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
- Updated FlightData spreadsheet as dates were no longer valid - Updated all findElements to FindBy in Homepage file - Added comments for visibility
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Nezic\IdeaProjects\CucumberIAG\src\test\java\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7544F2A-B3F6-4110-8B00-930F4C5944B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82110FDF-27E4-40AE-B930-0816F9325235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
   <si>
     <t>Flight Type</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Arrival location 1 does not match dataset</t>
-  </si>
-  <si>
     <t>No flight results</t>
   </si>
   <si>
@@ -166,15 +163,6 @@
     <t>Row 9 does not exist</t>
   </si>
   <si>
-    <t>₹1,22,140</t>
-  </si>
-  <si>
-    <t>₹8,368</t>
-  </si>
-  <si>
-    <t>₹1,30,518</t>
-  </si>
-  <si>
     <t>₹1,45,040</t>
   </si>
   <si>
@@ -208,15 +196,6 @@
     <t>1,073,452</t>
   </si>
   <si>
-    <t>24/01/2022 11:22:15 am</t>
-  </si>
-  <si>
-    <t>24/01/2022 11:22:22 am</t>
-  </si>
-  <si>
-    <t>24/01/2022 11:22:38 am</t>
-  </si>
-  <si>
     <t>24/01/2022 11:22:46 am</t>
   </si>
   <si>
@@ -238,9 +217,6 @@
     <t>24/01/2022 11:24:00 am</t>
   </si>
   <si>
-    <t>24/01/2022 1:40:21 pm</t>
-  </si>
-  <si>
     <t>24/01/2022 1:40:45 pm</t>
   </si>
   <si>
@@ -256,19 +232,22 @@
     <t>24/01/2022 1:41:07 pm</t>
   </si>
   <si>
-    <t>25/01/2022 1:51:28 pm</t>
-  </si>
-  <si>
-    <t>₹1,21,120</t>
-  </si>
-  <si>
-    <t>₹8,328</t>
-  </si>
-  <si>
-    <t>₹1,29,458</t>
-  </si>
-  <si>
-    <t>25/01/2022 2:23:05 pm</t>
+    <t>Departure date 1 does not match dataset</t>
+  </si>
+  <si>
+    <t>27/01/2022 10:25:48 am</t>
+  </si>
+  <si>
+    <t>27/01/2022 10:27:17 am</t>
+  </si>
+  <si>
+    <t>₹1,21,080</t>
+  </si>
+  <si>
+    <t>₹8,344</t>
+  </si>
+  <si>
+    <t>₹1,29,434</t>
   </si>
 </sst>
 </file>
@@ -656,7 +635,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -748,7 +727,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="3">
-        <v>25012022</v>
+        <v>25022022</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3">
@@ -826,7 +805,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="3">
-        <v>25012022</v>
+        <v>25022022</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="3">
@@ -871,7 +850,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="3">
-        <v>25012022</v>
+        <v>25022022</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3">
@@ -949,7 +928,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="3">
-        <v>25012022</v>
+        <v>25022022</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3">
@@ -1026,7 +1005,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
@@ -1035,21 +1014,21 @@
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
         <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -1058,21 +1037,21 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -1081,32 +1060,32 @@
         <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
@@ -1115,21 +1094,21 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
@@ -1138,60 +1117,60 @@
         <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Best practises update + testrun data
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Nezic\IdeaProjects\CucumberIAG\src\test\java\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82110FDF-27E4-40AE-B930-0816F9325235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF01EDF-9462-4648-B761-8D3B5E309E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t>Flight Type</t>
   </si>
@@ -163,15 +163,6 @@
     <t>Row 9 does not exist</t>
   </si>
   <si>
-    <t>₹1,45,040</t>
-  </si>
-  <si>
-    <t>₹10,360</t>
-  </si>
-  <si>
-    <t>₹1,55,410</t>
-  </si>
-  <si>
     <t>97,900</t>
   </si>
   <si>
@@ -196,65 +187,67 @@
     <t>1,073,452</t>
   </si>
   <si>
-    <t>24/01/2022 11:22:46 am</t>
-  </si>
-  <si>
-    <t>24/01/2022 11:22:59 am</t>
-  </si>
-  <si>
     <t>24/01/2022 11:23:15 am</t>
   </si>
   <si>
-    <t>24/01/2022 11:23:20 am</t>
-  </si>
-  <si>
-    <t>24/01/2022 11:23:30 am</t>
-  </si>
-  <si>
-    <t>24/01/2022 11:23:35 am</t>
-  </si>
-  <si>
-    <t>24/01/2022 11:24:00 am</t>
-  </si>
-  <si>
-    <t>24/01/2022 1:40:45 pm</t>
-  </si>
-  <si>
-    <t>₹23,990</t>
-  </si>
-  <si>
-    <t>₹3,761</t>
-  </si>
-  <si>
-    <t>₹27,761</t>
-  </si>
-  <si>
     <t>24/01/2022 1:41:07 pm</t>
   </si>
   <si>
-    <t>Departure date 1 does not match dataset</t>
-  </si>
-  <si>
-    <t>27/01/2022 10:25:48 am</t>
-  </si>
-  <si>
-    <t>27/01/2022 10:27:17 am</t>
-  </si>
-  <si>
-    <t>₹1,21,080</t>
-  </si>
-  <si>
-    <t>₹8,344</t>
-  </si>
-  <si>
-    <t>₹1,29,434</t>
+    <t>28/01/2022 12:46:35 pm</t>
+  </si>
+  <si>
+    <t>₹1,21,520</t>
+  </si>
+  <si>
+    <t>₹8,364</t>
+  </si>
+  <si>
+    <t>₹1,29,894</t>
+  </si>
+  <si>
+    <t>28/01/2022 12:46:55 pm</t>
+  </si>
+  <si>
+    <t>₹26,395</t>
+  </si>
+  <si>
+    <t>₹3,390</t>
+  </si>
+  <si>
+    <t>₹29,795</t>
+  </si>
+  <si>
+    <t>28/01/2022 12:48:09 pm</t>
+  </si>
+  <si>
+    <t>28/01/2022 12:48:36 pm</t>
+  </si>
+  <si>
+    <t>₹1,44,310</t>
+  </si>
+  <si>
+    <t>₹10,344</t>
+  </si>
+  <si>
+    <t>₹1,54,664</t>
+  </si>
+  <si>
+    <t>28/01/2022 12:49:19 pm</t>
+  </si>
+  <si>
+    <t>28/01/2022 12:49:30 pm</t>
+  </si>
+  <si>
+    <t>28/01/2022 12:49:34 pm</t>
+  </si>
+  <si>
+    <t>28/01/2022 12:49:44 pm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -635,28 +628,28 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" style="2" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="12.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="11.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="18.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="23.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="20.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
-    <col min="18" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -824,13 +817,13 @@
         <v>19</v>
       </c>
       <c r="M4" s="3">
-        <v>27012022</v>
+        <v>27022022</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="O4" s="3">
-        <v>28012022</v>
+        <v>28022022</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -970,14 +963,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="21.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="7.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="37.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="10.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="16.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="16.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="15.7109375" collapsed="true"/>
-    <col min="8" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1003,9 +996,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
@@ -1014,21 +1007,21 @@
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
         <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -1037,21 +1030,21 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -1060,21 +1053,21 @@
         <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
         <v>39</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
@@ -1085,7 +1078,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
@@ -1094,21 +1087,21 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
@@ -1117,43 +1110,43 @@
         <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
         <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
@@ -1164,7 +1157,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
- Made setData method static, removed unnecessary object creation as a result - Implemented ElementUtil to contain all selenium functions as per best practices - Updated keywords in feature file as per best practises
</commit_message>
<xml_diff>
--- a/src/test/java/Excel/FlightData.xlsx
+++ b/src/test/java/Excel/FlightData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Nezic\IdeaProjects\CucumberIAG\src\test\java\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF01EDF-9462-4648-B761-8D3B5E309E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C097C8AA-0FDE-4894-9391-6B2613E8C9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{15C5D190-8B55-41A7-AE81-1E037CBB6904}"/>
   </bookViews>
@@ -178,24 +178,9 @@
     <t>Row 7 does not exist</t>
   </si>
   <si>
-    <t>1,032,360</t>
-  </si>
-  <si>
-    <t>41,082</t>
-  </si>
-  <si>
-    <t>1,073,452</t>
-  </si>
-  <si>
     <t>24/01/2022 11:23:15 am</t>
   </si>
   <si>
-    <t>24/01/2022 1:41:07 pm</t>
-  </si>
-  <si>
-    <t>28/01/2022 12:46:35 pm</t>
-  </si>
-  <si>
     <t>₹1,21,520</t>
   </si>
   <si>
@@ -205,24 +190,12 @@
     <t>₹1,29,894</t>
   </si>
   <si>
-    <t>28/01/2022 12:46:55 pm</t>
-  </si>
-  <si>
-    <t>₹26,395</t>
-  </si>
-  <si>
     <t>₹3,390</t>
   </si>
   <si>
     <t>₹29,795</t>
   </si>
   <si>
-    <t>28/01/2022 12:48:09 pm</t>
-  </si>
-  <si>
-    <t>28/01/2022 12:48:36 pm</t>
-  </si>
-  <si>
     <t>₹1,44,310</t>
   </si>
   <si>
@@ -232,16 +205,43 @@
     <t>₹1,54,664</t>
   </si>
   <si>
-    <t>28/01/2022 12:49:19 pm</t>
-  </si>
-  <si>
-    <t>28/01/2022 12:49:30 pm</t>
-  </si>
-  <si>
-    <t>28/01/2022 12:49:34 pm</t>
-  </si>
-  <si>
-    <t>28/01/2022 12:49:44 pm</t>
+    <t>₹27,585</t>
+  </si>
+  <si>
+    <t>28/01/2022 2:23:14 pm</t>
+  </si>
+  <si>
+    <t>28/01/2022 2:23:32 pm</t>
+  </si>
+  <si>
+    <t>28/01/2022 2:24:02 pm</t>
+  </si>
+  <si>
+    <t>830,640</t>
+  </si>
+  <si>
+    <t>38,700</t>
+  </si>
+  <si>
+    <t>869,350</t>
+  </si>
+  <si>
+    <t>28/01/2022 2:24:37 pm</t>
+  </si>
+  <si>
+    <t>28/01/2022 2:24:51 pm</t>
+  </si>
+  <si>
+    <t>28/01/2022 2:25:21 pm</t>
+  </si>
+  <si>
+    <t>28/01/2022 2:25:27 pm</t>
+  </si>
+  <si>
+    <t>28/01/2022 2:25:43 pm</t>
+  </si>
+  <si>
+    <t>28/01/2022 2:25:48 pm</t>
   </si>
 </sst>
 </file>
@@ -628,7 +628,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -940,7 +940,7 @@
         <v>18</v>
       </c>
       <c r="M7" s="3">
-        <v>27012022</v>
+        <v>27022022</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -998,7 +998,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
@@ -1007,21 +1007,21 @@
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
         <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -1030,21 +1030,21 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -1053,21 +1053,21 @@
         <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
         <v>39</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
@@ -1087,21 +1087,21 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>

</xml_diff>